<commit_message>
Export excel FIN13 is 85% done
</commit_message>
<xml_diff>
--- a/public/Fin13.xlsx
+++ b/public/Fin13.xlsx
@@ -9,8 +9,6 @@
   <sheets>
     <sheet name="Hoja1. Actividades" sheetId="1" r:id="rId4"/>
     <sheet name="Hoja2. Integrantes" sheetId="2" r:id="rId5"/>
-    <sheet name="Hoja 3" sheetId="3" r:id="rId6"/>
-    <sheet name="Hoja3" sheetId="4" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="1" fullCalcOnLoad="0" forceFullCalc="0"/>
@@ -18,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="38">
   <si>
     <t>PLAN OPERATIVO DE GRUPOS Y SEMILLEROS DE INVESTIGACIÓN</t>
   </si>
@@ -32,12 +30,21 @@
     <t>NOMBRE DEL GRUPO Y/O SEMILLERO DE INVESTIGACIÓN</t>
   </si>
   <si>
+    <t>SIIC - Semillero de investigación en Inteligencia Computacional</t>
+  </si>
+  <si>
     <t>DIRECTOR DEL GRUPO Y/O SEMILLERO</t>
   </si>
   <si>
+    <t>Jose Alejandro Cortés Taborda</t>
+  </si>
+  <si>
     <t>SEMESTRE</t>
   </si>
   <si>
+    <t>2019-2</t>
+  </si>
+  <si>
     <t>ACTIVIDAD</t>
   </si>
   <si>
@@ -68,94 +75,58 @@
     <t>J</t>
   </si>
   <si>
+    <t>Primera actividad</t>
+  </si>
+  <si>
+    <t>Coordinador</t>
+  </si>
+  <si>
+    <t>FH05</t>
+  </si>
+  <si>
+    <t>Listado de asistencia</t>
+  </si>
+  <si>
+    <t>Primera actividad1</t>
+  </si>
+  <si>
+    <t>Primera actividad2</t>
+  </si>
+  <si>
+    <t>Primera actividad3</t>
+  </si>
+  <si>
+    <t>Primera actividad4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HORARIO DE REUNIÓN: </t>
+  </si>
+  <si>
+    <t>Codigo:FGI13</t>
+  </si>
+  <si>
+    <t>ACTUALIZAR INTEGRANTES</t>
+  </si>
+  <si>
+    <t>NOMBRE</t>
+  </si>
+  <si>
+    <t>CARGO (docente,estudiante, asesor)</t>
+  </si>
+  <si>
+    <t>CEDULA</t>
+  </si>
+  <si>
+    <t>TELEFONO</t>
+  </si>
+  <si>
+    <t>EMAIL (@elpoli.edu.co)</t>
+  </si>
+  <si>
+    <t>Estudiante</t>
+  </si>
+  <si>
     <t>jose_cortes82141@elpoli.edu.co</t>
-  </si>
-  <si>
-    <t>HORARIO DE REUNIÓN: VIERNES DE 4.6PM BLOQUE P13-305</t>
-  </si>
-  <si>
-    <t>Codigo:FGI13</t>
-  </si>
-  <si>
-    <t>ACTUALIZAR INTEGRANTES</t>
-  </si>
-  <si>
-    <t>NOMBRE</t>
-  </si>
-  <si>
-    <t>CARGO (docente,estudiante, asesor)</t>
-  </si>
-  <si>
-    <t>CEDULA</t>
-  </si>
-  <si>
-    <t>TELEFONO</t>
-  </si>
-  <si>
-    <t>EMAIL (@elpoli.edu.co)</t>
-  </si>
-  <si>
-    <t>Sandra P. Mateus</t>
-  </si>
-  <si>
-    <t>docente</t>
-  </si>
-  <si>
-    <t>ext 477</t>
-  </si>
-  <si>
-    <t>spmateus</t>
-  </si>
-  <si>
-    <t>Jorge E. Giraldo Plaza</t>
-  </si>
-  <si>
-    <t>ext 484</t>
-  </si>
-  <si>
-    <t>jegiraldo</t>
-  </si>
-  <si>
-    <t>Jorge E. Espinosa</t>
-  </si>
-  <si>
-    <t>ext 457</t>
-  </si>
-  <si>
-    <t>jeespinosa</t>
-  </si>
-  <si>
-    <t>David Montoya Perez</t>
-  </si>
-  <si>
-    <t>estudiante</t>
-  </si>
-  <si>
-    <t>david_montoya82131</t>
-  </si>
-  <si>
-    <t>Santiago Suarez</t>
-  </si>
-  <si>
-    <t>santiago_suarez82111</t>
-  </si>
-  <si>
-    <t>Daniel Ramos Bolivar</t>
-  </si>
-  <si>
-    <t>daniel_ramos82103</t>
-  </si>
-  <si>
-    <t>Steven Suarez Cano</t>
-  </si>
-  <si>
-    <t>steven_suarez82102</t>
-  </si>
-  <si>
-    <t>Jovany albeiro lopez zapata</t>
-  </si>
-  <si>
-    <t>Jovany_lopez82101</t>
   </si>
   <si>
     <r>
@@ -173,60 +144,6 @@
       </rPr>
       <t xml:space="preserve"> diligencie los integrantes activos al inicio del semestre del informe</t>
     </r>
-  </si>
-  <si>
-    <t>S</t>
-  </si>
-  <si>
-    <t>O</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>Presentación Semillero</t>
-  </si>
-  <si>
-    <t>Coordinador</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>Capacitación consulta a bases de datos y herramientas</t>
-  </si>
-  <si>
-    <t>Revisión de tendencias en áreas de interés</t>
-  </si>
-  <si>
-    <t>Estudiantes</t>
-  </si>
-  <si>
-    <t>Revisión avances de Trabajos de Grado</t>
-  </si>
-  <si>
-    <t>Identificación Problemáticas en áreas de interés</t>
-  </si>
-  <si>
-    <t>Definición de micro-Proyectos</t>
-  </si>
-  <si>
-    <t>Documentación de micro-Proyectos</t>
-  </si>
-  <si>
-    <t>Socialización de micro-Proyectos</t>
-  </si>
-  <si>
-    <t>capacitación propuesta por estudiantes</t>
-  </si>
-  <si>
-    <t>Revisión avances micro-Proyecto</t>
-  </si>
-  <si>
-    <t>Reunión final</t>
   </si>
 </sst>
 </file>
@@ -459,9 +376,9 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>199885</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>28277</xdr:rowOff>
+      <xdr:rowOff>30510</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="666750" cy="333375"/>
+    <xdr:ext cx="666750" cy="323850"/>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="1" name="" descr=""/>
@@ -487,11 +404,11 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>657634</xdr:colOff>
+      <xdr:colOff>656695</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:rowOff>145107</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="1428750" cy="685800"/>
+    <xdr:ext cx="1447800" cy="676275"/>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="2" name="" descr=""/>
@@ -522,46 +439,11 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>552859</xdr:colOff>
+      <xdr:colOff>555222</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>66973</xdr:rowOff>
+      <xdr:rowOff>68461</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="447675" cy="285750"/>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="1" name="" descr=""/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm rot="0"/>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>199885</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>28277</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="666750" cy="333375"/>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="1" name="" descr=""/>
@@ -880,7 +762,7 @@
   <dimension ref="A1:CK1093"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="E4" sqref="E4:J4"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="true" defaultRowHeight="15" defaultColWidth="10" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1013,7 +895,9 @@
       <c r="B4" s="13"/>
       <c r="C4" s="13"/>
       <c r="D4" s="14"/>
-      <c r="E4" s="11"/>
+      <c r="E4" s="11" t="s">
+        <v>4</v>
+      </c>
       <c r="F4" s="11"/>
       <c r="G4" s="11"/>
       <c r="H4" s="11"/>
@@ -1022,12 +906,14 @@
     </row>
     <row r="5" spans="1:89" customHeight="1" ht="15">
       <c r="A5" s="15" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" s="15"/>
       <c r="C5" s="15"/>
       <c r="D5" s="15"/>
-      <c r="E5" s="11"/>
+      <c r="E5" s="11" t="s">
+        <v>6</v>
+      </c>
       <c r="F5" s="11"/>
       <c r="G5" s="11"/>
       <c r="H5" s="11"/>
@@ -1036,12 +922,14 @@
     </row>
     <row r="6" spans="1:89" customHeight="1" ht="15">
       <c r="A6" s="15" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B6" s="15"/>
       <c r="C6" s="15"/>
       <c r="D6" s="15"/>
-      <c r="E6" s="11"/>
+      <c r="E6" s="11" t="s">
+        <v>8</v>
+      </c>
       <c r="F6" s="11"/>
       <c r="G6" s="11"/>
       <c r="H6" s="11"/>
@@ -1050,26 +938,26 @@
     </row>
     <row r="8" spans="1:89" customHeight="1" ht="14.25">
       <c r="A8" s="17" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E8" s="17"/>
       <c r="F8" s="17"/>
       <c r="G8" s="17"/>
       <c r="H8" s="17"/>
       <c r="I8" s="17" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="J8" s="17" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:89" customHeight="1" ht="15">
@@ -1077,84 +965,122 @@
       <c r="B9" s="17"/>
       <c r="C9" s="17"/>
       <c r="D9" s="4" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="I9" s="17"/>
       <c r="J9" s="17"/>
     </row>
     <row r="10" spans="1:89" customHeight="1" ht="15">
       <c r="A10" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="2"/>
+        <v>19</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
+      <c r="I10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="11" spans="1:89" customHeight="1" ht="15">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
+      <c r="A11" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
+      <c r="I11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="12" spans="1:89" customHeight="1" ht="15">
-      <c r="A12" s="9"/>
-      <c r="B12" s="2"/>
+      <c r="A12" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
+      <c r="I12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="13" spans="1:89" customHeight="1" ht="15">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
+      <c r="A13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
+      <c r="I13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="14" spans="1:89" customHeight="1" ht="15">
-      <c r="A14" s="9"/>
-      <c r="B14" s="2"/>
+      <c r="A14" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
+      <c r="I14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="15" spans="1:89" customHeight="1" ht="15">
       <c r="A15" s="2"/>
@@ -1258,7 +1184,7 @@
     <row r="24" spans="1:89" customHeight="1" ht="15" s="5" customFormat="1"/>
     <row r="25" spans="1:89" customHeight="1" ht="18.75" s="5" customFormat="1">
       <c r="A25" s="10" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
     </row>
     <row r="26" spans="1:89" customHeight="1" ht="15" s="5" customFormat="1"/>
@@ -2370,7 +2296,7 @@
   <dimension ref="A1:AS384"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="true" defaultRowHeight="15" defaultColWidth="10" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2379,7 +2305,7 @@
     <col min="2" max="2" width="19.42578125" customWidth="true" style="1"/>
     <col min="3" max="3" width="15.140625" customWidth="true" style="0"/>
     <col min="4" max="4" width="14.28515625" customWidth="true" style="0"/>
-    <col min="5" max="5" width="25.5703125" customWidth="true" style="0"/>
+    <col min="5" max="5" width="28.140625" customWidth="true" style="0"/>
     <col min="7" max="7" width="11.42578125" customWidth="true" style="5"/>
     <col min="8" max="8" width="11.42578125" customWidth="true" style="5"/>
     <col min="9" max="9" width="11.42578125" customWidth="true" style="5"/>
@@ -2429,7 +2355,7 @@
       <c r="C1" s="16"/>
       <c r="D1" s="16"/>
       <c r="E1" s="2" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="F1" s="8"/>
       <c r="G1" s="8"/>
@@ -2562,7 +2488,7 @@
     </row>
     <row r="4" spans="1:45" customHeight="1" ht="15">
       <c r="A4" s="18" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="B4" s="18"/>
       <c r="C4" s="18"/>
@@ -2571,116 +2497,72 @@
     </row>
     <row r="5" spans="1:45" customHeight="1" ht="38.25">
       <c r="A5" s="6" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:45" customHeight="1" ht="15">
       <c r="A6" s="7" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7" t="s">
-        <v>27</v>
+        <v>35</v>
+      </c>
+      <c r="C6" s="7">
+        <v>1035</v>
+      </c>
+      <c r="D6" s="7">
+        <v>12</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:45" customHeight="1" ht="15">
-      <c r="A7" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>26</v>
-      </c>
+      <c r="A7" s="7"/>
+      <c r="B7" s="7"/>
       <c r="C7" s="7"/>
-      <c r="D7" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>31</v>
-      </c>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
     </row>
     <row r="8" spans="1:45" customHeight="1" ht="15">
-      <c r="A8" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>26</v>
-      </c>
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
       <c r="C8" s="7"/>
-      <c r="D8" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>34</v>
-      </c>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
     </row>
     <row r="9" spans="1:45" customHeight="1" ht="15">
-      <c r="A9" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C9" s="7">
-        <v>1020469704</v>
-      </c>
-      <c r="D9" s="7">
-        <v>3146399636</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>37</v>
-      </c>
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
     </row>
     <row r="10" spans="1:45" customHeight="1" ht="15">
-      <c r="A10" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C10" s="7">
-        <v>1017206051</v>
-      </c>
-      <c r="D10" s="7">
-        <v>3014455684</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>39</v>
-      </c>
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
     </row>
     <row r="11" spans="1:45" customHeight="1" ht="15" s="1" customFormat="1">
-      <c r="A11" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C11" s="7">
-        <v>1128282099</v>
-      </c>
-      <c r="D11" s="7">
-        <v>3022313748</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>41</v>
-      </c>
+      <c r="A11" s="7"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
@@ -2722,21 +2604,11 @@
       <c r="AS11" s="5"/>
     </row>
     <row r="12" spans="1:45" customHeight="1" ht="15" s="1" customFormat="1">
-      <c r="A12" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C12" s="7">
-        <v>1040739738</v>
-      </c>
-      <c r="D12" s="7">
-        <v>3207116222</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>43</v>
-      </c>
+      <c r="A12" s="7"/>
+      <c r="B12" s="7"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
@@ -2778,21 +2650,11 @@
       <c r="AS12" s="5"/>
     </row>
     <row r="13" spans="1:45" customHeight="1" ht="15" s="1" customFormat="1">
-      <c r="A13" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" s="7">
-        <v>1128407669</v>
-      </c>
-      <c r="D13" s="7">
-        <v>3015053204</v>
-      </c>
-      <c r="E13" s="7" t="s">
-        <v>45</v>
-      </c>
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
@@ -2902,7 +2764,7 @@
     </row>
     <row r="18" spans="1:45" customHeight="1" ht="15">
       <c r="A18" s="3" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="B18" s="3"/>
     </row>
@@ -3291,1569 +3153,4 @@
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
-  <dimension ref="A1:CH1097"/>
-  <sheetViews>
-    <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="N13" sqref="N13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr customHeight="true" defaultRowHeight="15" defaultColWidth="11.42578125" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col min="1" max="1" width="53.85546875" customWidth="true" style="1"/>
-    <col min="2" max="2" width="16.28515625" customWidth="true" style="1"/>
-    <col min="3" max="3" width="3.140625" customWidth="true" style="1"/>
-    <col min="4" max="4" width="2.7109375" customWidth="true" style="1"/>
-    <col min="5" max="5" width="2.7109375" customWidth="true" style="1"/>
-    <col min="6" max="6" width="2.85546875" customWidth="true" style="1"/>
-    <col min="7" max="7" width="3" customWidth="true" style="1"/>
-    <col min="8" max="8" width="4.42578125" customWidth="true" style="5"/>
-    <col min="9" max="9" width="11.42578125" style="5"/>
-    <col min="10" max="10" width="11.42578125" style="5"/>
-    <col min="11" max="11" width="11.42578125" style="5"/>
-    <col min="12" max="12" width="11.42578125" style="5"/>
-    <col min="13" max="13" width="11.42578125" style="5"/>
-    <col min="14" max="14" width="11.42578125" style="5"/>
-    <col min="15" max="15" width="11.42578125" style="5"/>
-    <col min="16" max="16" width="11.42578125" style="5"/>
-    <col min="17" max="17" width="11.42578125" style="5"/>
-    <col min="18" max="18" width="11.42578125" style="5"/>
-    <col min="19" max="19" width="11.42578125" style="5"/>
-    <col min="20" max="20" width="11.42578125" style="5"/>
-    <col min="21" max="21" width="11.42578125" style="5"/>
-    <col min="22" max="22" width="11.42578125" style="5"/>
-    <col min="23" max="23" width="11.42578125" style="5"/>
-    <col min="24" max="24" width="11.42578125" style="5"/>
-    <col min="25" max="25" width="11.42578125" style="5"/>
-    <col min="26" max="26" width="11.42578125" style="5"/>
-    <col min="27" max="27" width="11.42578125" style="5"/>
-    <col min="28" max="28" width="11.42578125" style="5"/>
-    <col min="29" max="29" width="11.42578125" style="5"/>
-    <col min="30" max="30" width="11.42578125" style="5"/>
-    <col min="31" max="31" width="11.42578125" style="5"/>
-    <col min="32" max="32" width="11.42578125" style="5"/>
-    <col min="33" max="33" width="11.42578125" style="5"/>
-    <col min="34" max="34" width="11.42578125" style="5"/>
-    <col min="35" max="35" width="11.42578125" style="5"/>
-    <col min="36" max="36" width="11.42578125" style="5"/>
-    <col min="37" max="37" width="11.42578125" style="5"/>
-    <col min="38" max="38" width="11.42578125" style="5"/>
-    <col min="39" max="39" width="11.42578125" style="5"/>
-    <col min="40" max="40" width="11.42578125" style="5"/>
-    <col min="41" max="41" width="11.42578125" style="5"/>
-    <col min="42" max="42" width="11.42578125" style="5"/>
-    <col min="43" max="43" width="11.42578125" style="5"/>
-    <col min="44" max="44" width="11.42578125" style="5"/>
-    <col min="45" max="45" width="11.42578125" style="5"/>
-    <col min="46" max="46" width="11.42578125" style="5"/>
-    <col min="47" max="47" width="11.42578125" style="5"/>
-    <col min="48" max="48" width="11.42578125" style="5"/>
-    <col min="49" max="49" width="11.42578125" style="5"/>
-    <col min="50" max="50" width="11.42578125" style="5"/>
-    <col min="51" max="51" width="11.42578125" style="5"/>
-    <col min="52" max="52" width="11.42578125" style="5"/>
-    <col min="53" max="53" width="11.42578125" style="5"/>
-    <col min="54" max="54" width="11.42578125" style="5"/>
-    <col min="55" max="55" width="11.42578125" style="5"/>
-    <col min="56" max="56" width="11.42578125" style="5"/>
-    <col min="57" max="57" width="11.42578125" style="5"/>
-    <col min="58" max="58" width="11.42578125" style="5"/>
-    <col min="59" max="59" width="11.42578125" style="5"/>
-    <col min="60" max="60" width="11.42578125" style="5"/>
-    <col min="61" max="61" width="11.42578125" style="5"/>
-    <col min="62" max="62" width="11.42578125" style="5"/>
-    <col min="63" max="63" width="11.42578125" style="5"/>
-    <col min="64" max="64" width="11.42578125" style="5"/>
-    <col min="65" max="65" width="11.42578125" style="5"/>
-    <col min="66" max="66" width="11.42578125" style="5"/>
-    <col min="67" max="67" width="11.42578125" style="5"/>
-    <col min="68" max="68" width="11.42578125" style="5"/>
-    <col min="69" max="69" width="11.42578125" style="5"/>
-    <col min="70" max="70" width="11.42578125" style="5"/>
-    <col min="71" max="71" width="11.42578125" style="5"/>
-    <col min="72" max="72" width="11.42578125" style="5"/>
-    <col min="73" max="73" width="11.42578125" style="5"/>
-    <col min="74" max="74" width="11.42578125" style="5"/>
-    <col min="75" max="75" width="11.42578125" style="5"/>
-    <col min="76" max="76" width="11.42578125" style="5"/>
-    <col min="77" max="77" width="11.42578125" style="5"/>
-    <col min="78" max="78" width="11.42578125" style="5"/>
-    <col min="79" max="79" width="11.42578125" style="5"/>
-    <col min="80" max="80" width="11.42578125" style="5"/>
-    <col min="81" max="81" width="11.42578125" style="5"/>
-    <col min="82" max="82" width="11.42578125" style="5"/>
-    <col min="83" max="83" width="11.42578125" style="5"/>
-    <col min="84" max="84" width="11.42578125" style="5"/>
-    <col min="85" max="85" width="11.42578125" style="5"/>
-    <col min="86" max="86" width="11.42578125" style="5"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:86" customHeight="1" ht="15">
-      <c r="A1" s="11"/>
-      <c r="B1" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-    </row>
-    <row r="2" spans="1:86" customHeight="1" ht="17.25">
-      <c r="A2" s="11"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-    </row>
-    <row r="4" spans="1:86" customHeight="1" ht="14.25" s="5" customFormat="1">
-      <c r="A4" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-    </row>
-    <row r="5" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1">
-      <c r="A5" s="17"/>
-      <c r="B5" s="17"/>
-      <c r="C5" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1">
-      <c r="A6" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-    </row>
-    <row r="7" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1">
-      <c r="A7" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-    </row>
-    <row r="8" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1">
-      <c r="A8" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-    </row>
-    <row r="9" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1">
-      <c r="A9" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-    </row>
-    <row r="10" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1">
-      <c r="A10" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-    </row>
-    <row r="11" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1">
-      <c r="A11" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-    </row>
-    <row r="12" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1">
-      <c r="A12" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-    </row>
-    <row r="13" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1">
-      <c r="A13" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-    </row>
-    <row r="14" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1">
-      <c r="A14" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-    </row>
-    <row r="15" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1">
-      <c r="A15" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-    </row>
-    <row r="16" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1">
-      <c r="A16" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="G16" s="2"/>
-    </row>
-    <row r="17" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1">
-      <c r="A17" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="G17" s="2"/>
-    </row>
-    <row r="18" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1">
-      <c r="A18" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="G18" s="2"/>
-    </row>
-    <row r="19" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1">
-      <c r="A19" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="G19" s="2"/>
-    </row>
-    <row r="20" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1">
-      <c r="A20" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="21" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-    </row>
-    <row r="22" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
-    </row>
-    <row r="23" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-    </row>
-    <row r="24" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-    </row>
-    <row r="25" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
-    </row>
-    <row r="26" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1">
-      <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-    </row>
-    <row r="27" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-    </row>
-    <row r="28" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="29" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="30" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="31" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="32" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="33" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="34" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="35" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="36" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="37" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="38" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="39" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="40" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="41" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="42" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="43" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="44" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="45" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="46" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="47" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="48" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="49" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="50" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="51" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="52" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="53" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="54" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="55" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="56" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="57" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="58" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="59" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="60" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="61" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="62" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="63" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="64" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="65" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="66" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="67" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="68" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="69" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="70" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="71" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="72" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="73" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="74" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="75" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="76" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="77" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="78" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="79" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="80" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="81" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="82" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="83" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="84" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="85" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="86" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="87" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="88" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="89" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="90" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="91" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="92" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="93" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="94" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="95" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="96" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="97" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="98" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="99" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="100" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="101" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="102" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="103" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="104" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="105" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="106" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="107" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="108" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="109" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="110" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="111" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="112" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="113" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="114" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="115" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="116" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="117" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="118" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="119" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="120" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="121" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="122" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="123" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="124" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="125" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="126" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="127" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="128" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="129" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="130" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="131" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="132" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="133" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="134" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="135" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="136" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="137" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="138" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="139" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="140" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="141" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="142" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="143" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="144" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="145" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="146" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="147" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="148" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="149" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="150" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="151" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="152" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="153" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="154" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="155" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="156" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="157" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="158" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="159" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="160" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="161" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="162" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="163" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="164" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="165" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="166" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="167" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="168" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="169" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="170" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="171" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="172" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="173" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="174" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="175" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="176" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="177" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="178" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="179" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="180" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="181" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="182" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="183" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="184" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="185" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="186" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="187" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="188" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="189" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="190" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="191" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="192" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="193" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="194" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="195" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="196" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="197" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="198" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="199" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="200" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="201" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="202" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="203" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="204" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="205" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="206" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="207" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="208" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="209" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="210" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="211" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="212" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="213" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="214" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="215" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="216" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="217" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="218" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="219" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="220" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="221" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="222" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="223" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="224" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="225" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="226" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="227" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="228" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="229" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="230" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="231" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="232" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="233" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="234" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="235" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="236" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="237" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="238" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="239" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="240" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="241" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="242" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="243" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="244" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="245" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="246" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="247" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="248" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="249" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="250" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="251" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="252" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="253" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="254" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="255" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="256" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="257" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="258" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="259" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="260" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="261" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="262" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="263" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="264" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="265" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="266" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="267" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="268" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="269" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="270" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="271" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="272" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="273" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="274" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="275" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="276" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="277" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="278" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="279" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="280" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="281" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="282" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="283" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="284" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="285" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="286" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="287" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="288" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="289" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="290" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="291" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="292" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="293" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="294" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="295" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="296" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="297" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="298" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="299" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="300" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="301" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="302" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="303" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="304" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="305" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="306" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="307" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="308" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="309" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="310" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="311" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="312" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="313" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="314" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="315" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="316" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="317" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="318" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="319" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="320" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="321" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="322" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="323" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="324" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="325" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="326" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="327" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="328" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="329" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="330" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="331" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="332" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="333" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="334" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="335" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="336" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="337" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="338" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="339" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="340" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="341" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="342" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="343" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="344" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="345" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="346" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="347" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="348" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="349" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="350" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="351" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="352" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="353" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="354" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="355" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="356" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="357" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="358" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="359" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="360" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="361" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="362" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="363" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="364" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="365" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="366" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="367" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="368" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="369" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="370" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="371" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="372" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="373" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="374" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="375" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="376" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="377" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="378" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="379" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="380" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="381" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="382" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="383" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="384" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="385" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="386" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="387" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="388" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="389" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="390" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="391" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="392" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="393" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="394" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="395" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="396" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="397" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="398" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="399" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="400" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="401" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="402" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="403" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="404" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="405" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="406" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="407" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="408" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="409" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="410" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="411" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="412" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="413" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="414" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="415" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="416" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="417" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="418" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="419" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="420" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="421" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="422" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="423" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="424" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="425" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="426" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="427" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="428" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="429" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="430" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="431" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="432" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="433" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="434" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="435" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="436" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="437" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="438" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="439" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="440" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="441" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="442" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="443" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="444" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="445" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="446" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="447" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="448" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="449" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="450" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="451" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="452" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="453" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="454" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="455" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="456" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="457" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="458" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="459" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="460" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="461" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="462" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="463" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="464" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="465" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="466" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="467" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="468" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="469" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="470" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="471" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="472" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="473" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="474" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="475" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="476" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="477" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="478" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="479" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="480" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="481" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="482" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="483" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="484" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="485" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="486" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="487" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="488" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="489" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="490" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="491" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="492" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="493" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="494" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="495" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="496" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="497" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="498" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="499" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="500" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="501" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="502" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="503" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="504" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="505" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="506" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="507" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="508" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="509" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="510" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="511" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="512" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="513" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="514" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="515" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="516" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="517" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="518" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="519" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="520" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="521" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="522" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="523" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="524" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="525" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="526" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="527" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="528" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="529" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="530" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="531" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="532" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="533" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="534" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="535" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="536" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="537" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="538" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="539" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="540" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="541" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="542" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="543" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="544" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="545" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="546" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="547" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="548" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="549" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="550" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="551" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="552" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="553" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="554" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="555" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="556" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="557" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="558" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="559" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="560" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="561" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="562" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="563" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="564" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="565" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="566" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="567" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="568" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="569" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="570" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="571" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="572" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="573" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="574" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="575" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="576" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="577" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="578" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="579" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="580" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="581" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="582" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="583" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="584" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="585" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="586" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="587" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="588" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="589" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="590" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="591" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="592" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="593" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="594" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="595" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="596" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="597" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="598" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="599" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="600" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="601" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="602" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="603" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="604" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="605" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="606" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="607" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="608" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="609" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="610" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="611" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="612" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="613" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="614" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="615" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="616" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="617" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="618" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="619" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="620" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="621" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="622" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="623" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="624" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="625" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="626" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="627" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="628" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="629" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="630" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="631" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="632" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="633" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="634" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="635" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="636" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="637" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="638" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="639" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="640" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="641" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="642" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="643" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="644" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="645" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="646" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="647" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="648" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="649" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="650" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="651" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="652" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="653" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="654" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="655" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="656" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="657" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="658" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="659" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="660" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="661" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="662" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="663" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="664" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="665" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="666" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="667" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="668" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="669" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="670" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="671" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="672" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="673" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="674" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="675" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="676" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="677" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="678" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="679" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="680" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="681" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="682" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="683" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="684" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="685" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="686" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="687" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="688" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="689" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="690" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="691" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="692" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="693" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="694" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="695" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="696" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="697" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="698" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="699" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="700" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="701" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="702" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="703" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="704" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="705" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="706" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="707" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="708" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="709" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="710" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="711" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="712" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="713" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="714" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="715" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="716" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="717" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="718" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="719" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="720" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="721" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="722" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="723" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="724" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="725" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="726" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="727" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="728" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="729" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="730" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="731" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="732" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="733" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="734" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="735" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="736" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="737" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="738" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="739" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="740" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="741" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="742" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="743" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="744" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="745" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="746" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="747" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="748" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="749" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="750" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="751" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="752" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="753" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="754" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="755" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="756" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="757" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="758" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="759" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="760" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="761" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="762" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="763" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="764" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="765" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="766" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="767" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="768" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="769" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="770" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="771" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="772" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="773" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="774" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="775" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="776" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="777" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="778" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="779" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="780" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="781" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="782" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="783" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="784" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="785" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="786" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="787" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="788" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="789" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="790" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="791" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="792" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="793" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="794" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="795" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="796" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="797" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="798" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="799" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="800" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="801" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="802" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="803" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="804" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="805" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="806" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="807" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="808" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="809" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="810" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="811" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="812" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="813" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="814" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="815" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="816" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="817" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="818" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="819" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="820" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="821" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="822" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="823" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="824" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="825" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="826" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="827" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="828" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="829" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="830" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="831" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="832" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="833" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="834" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="835" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="836" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="837" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="838" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="839" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="840" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="841" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="842" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="843" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="844" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="845" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="846" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="847" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="848" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="849" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="850" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="851" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="852" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="853" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="854" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="855" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="856" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="857" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="858" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="859" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="860" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="861" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="862" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="863" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="864" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="865" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="866" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="867" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="868" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="869" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="870" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="871" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="872" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="873" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="874" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="875" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="876" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="877" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="878" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="879" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="880" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="881" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="882" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="883" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="884" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="885" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="886" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="887" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="888" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="889" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="890" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="891" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="892" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="893" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="894" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="895" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="896" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="897" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="898" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="899" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="900" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="901" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="902" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="903" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="904" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="905" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="906" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="907" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="908" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="909" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="910" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="911" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="912" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="913" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="914" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="915" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="916" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="917" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="918" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="919" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="920" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="921" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="922" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="923" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="924" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="925" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="926" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="927" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="928" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="929" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="930" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="931" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="932" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="933" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="934" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="935" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="936" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="937" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="938" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="939" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="940" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="941" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="942" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="943" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="944" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="945" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="946" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="947" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="948" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="949" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="950" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="951" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="952" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="953" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="954" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="955" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="956" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="957" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="958" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="959" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="960" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="961" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="962" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="963" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="964" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="965" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="966" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="967" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="968" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="969" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="970" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="971" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="972" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="973" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="974" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="975" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="976" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="977" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="978" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="979" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="980" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="981" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="982" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="983" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="984" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="985" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="986" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="987" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="988" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="989" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="990" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="991" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="992" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="993" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="994" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="995" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="996" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="997" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="998" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="999" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1000" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1001" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1002" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1003" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1004" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1005" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1006" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1007" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1008" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1009" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1010" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1011" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1012" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1013" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1014" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1015" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1016" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1017" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1018" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1019" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1020" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1021" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1022" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1023" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1024" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1025" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1026" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1027" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1028" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1029" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1030" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1031" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1032" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1033" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1034" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1035" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1036" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1037" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1038" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1039" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1040" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1041" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1042" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1043" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1044" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1045" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1046" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1047" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1048" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1049" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1050" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1051" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1052" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1053" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1054" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1055" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1056" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1057" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1058" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1059" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1060" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1061" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1062" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1063" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1064" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1065" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1066" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1067" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1068" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1069" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1070" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1071" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1072" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1073" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1074" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1075" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1076" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1077" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1078" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1079" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1080" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1081" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1082" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1083" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1084" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1085" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1086" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1087" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1088" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1089" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1090" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1091" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1092" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1093" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1094" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1095" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1096" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-    <row r="1097" spans="1:86" customHeight="1" ht="15" s="5" customFormat="1"/>
-  </sheetData>
-  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="true" formatColumns="true" formatRows="true" insertColumns="true" insertRows="true" insertHyperlinks="true" deleteColumns="true" deleteRows="true" selectLockedCells="false" sort="true" autoFilter="true" pivotTables="true" selectUnlockedCells="false"/>
-  <mergeCells>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:G4"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:G2"/>
-  </mergeCells>
-  <printOptions gridLines="false" gridLinesSet="true"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait" scale="100" fitToHeight="1" fitToWidth="1"/>
-  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader/>
-    <oddFooter/>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr customHeight="true" defaultRowHeight="15" defaultColWidth="10" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData/>
-  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="true" formatColumns="true" formatRows="true" insertColumns="true" insertRows="true" insertHyperlinks="true" deleteColumns="true" deleteRows="true" selectLockedCells="false" sort="true" autoFilter="true" pivotTables="true" selectUnlockedCells="false"/>
-  <printOptions gridLines="false" gridLinesSet="true"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1"/>
-  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader/>
-    <oddFooter/>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
-</worksheet>
 </file>
</xml_diff>